<commit_message>
vault backup: 2023-12-02 23:35:39
</commit_message>
<xml_diff>
--- a/ME 436/Labs/Heat Pump/Data 33F.xlsx
+++ b/ME 436/Labs/Heat Pump/Data 33F.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lab Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mania\Desktop\ME_Fall_2023\ME 436\Labs\Heat Pump\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08258DC-38FB-47AC-A2B2-925BC10A6F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11EB07D-8499-492F-B026-766D67E4FA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="380" windowWidth="29020" windowHeight="15820" xr2:uid="{A8AB8957-7FBA-4282-BCDA-67C24621813A}"/>
+    <workbookView xWindow="14295" yWindow="7740" windowWidth="14610" windowHeight="7845" xr2:uid="{A8AB8957-7FBA-4282-BCDA-67C24621813A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,10 @@
     <t>Condenser Outlet Pressure</t>
   </si>
   <si>
-    <t>Ondenser Outlet Temperature</t>
+    <t>Outdoor Temperature</t>
   </si>
   <si>
-    <t>Outdoor Temperature</t>
+    <t>Condenser Outlet Temperature</t>
   </si>
 </sst>
 </file>
@@ -422,23 +422,24 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.08984375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="28.81640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +450,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -464,10 +465,10 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>32.581000000000003</v>
       </c>
@@ -496,7 +497,7 @@
         <v>104.41500000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>32.533000000000001</v>
       </c>
@@ -525,7 +526,7 @@
         <v>104.443</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>32.481999999999999</v>
       </c>
@@ -554,7 +555,7 @@
         <v>104.462</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>32.439</v>
       </c>
@@ -583,7 +584,7 @@
         <v>104.49</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>32.401000000000003</v>
       </c>
@@ -612,7 +613,7 @@
         <v>104.504</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>32.368000000000002</v>
       </c>
@@ -641,7 +642,7 @@
         <v>104.53700000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>32.326000000000001</v>
       </c>
@@ -670,7 +671,7 @@
         <v>104.556</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>32.279000000000003</v>
       </c>
@@ -699,7 +700,7 @@
         <v>104.56100000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>32.241</v>
       </c>
@@ -728,7 +729,7 @@
         <v>104.59399999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>32.203000000000003</v>
       </c>
@@ -757,7 +758,7 @@
         <v>104.608</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>32.165999999999997</v>
       </c>
@@ -786,7 +787,7 @@
         <v>104.636</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>32.142000000000003</v>
       </c>
@@ -815,7 +816,7 @@
         <v>104.66500000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>32.118000000000002</v>
       </c>
@@ -844,7 +845,7 @@
         <v>104.693</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>32.070999999999998</v>
       </c>
@@ -873,7 +874,7 @@
         <v>104.721</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>33.381999999999998</v>
       </c>
@@ -902,7 +903,7 @@
         <v>104.764</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>33.335000000000001</v>
       </c>
@@ -931,7 +932,7 @@
         <v>104.78700000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>33.307000000000002</v>
       </c>
@@ -960,7 +961,7 @@
         <v>104.825</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>33.255000000000003</v>
       </c>
@@ -989,7 +990,7 @@
         <v>104.863</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>33.213000000000001</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>104.901</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>33.164999999999999</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>104.934</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>33.405999999999999</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>104.95699999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>33.381999999999998</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>104.99</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>33.335000000000001</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>105.033</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>33.307000000000002</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>105.066</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>33.255000000000003</v>
       </c>
@@ -1192,7 +1193,7 @@
         <v>105.084</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>33.213000000000001</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>105.113</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>33.164999999999999</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>105.127</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>33.122999999999998</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>105.155</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>33.070999999999998</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>105.169</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>33.029000000000003</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>105.19799999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32.972000000000001</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>105.221</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32.914999999999999</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>105.71599999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32.878</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>106.212</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32.820999999999998</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>106.70699999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32.779000000000003</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>107.202</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>32.741</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>107.70699999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>32.698999999999998</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>108.197</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>32.655999999999999</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>108.68300000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32.622999999999998</v>
       </c>
@@ -1598,7 +1599,7 @@
         <v>109.16800000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>32.581000000000003</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>109.654</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>32.533000000000001</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>110.14</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>32.682000000000002</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>110.14</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>32.639000000000003</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>110.14</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>32.600999999999999</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>110.149</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>32.667999999999999</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>110.154</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>32.625999999999998</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>110.154</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>32.679000000000002</v>
       </c>
@@ -1830,7 +1831,7 @@
         <v>110.16800000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>32.640999999999998</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>110.182</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>32.603000000000002</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>110.20099999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>32.665999999999997</v>
       </c>
@@ -1917,7 +1918,7 @@
         <v>110.23</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>32.642000000000003</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>110.248</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>32.618000000000002</v>
       </c>
@@ -1975,7 +1976,7 @@
         <v>110.267</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>32.670999999999999</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>110.286</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>32.624000000000002</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>110.30500000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>32.686</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>110.32899999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>32.963000000000001</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>110.34699999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>32.93</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>110.36199999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>32.892000000000003</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>110.376</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>32.859000000000002</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>110.38500000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>32.826000000000001</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>110.366</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>32.787999999999997</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>110.366</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>32.750999999999998</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>110.366</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>32.726999999999997</v>
       </c>
@@ -2294,7 +2295,7 @@
         <v>110.371</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>32.694000000000003</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>110.376</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>32.661000000000001</v>
       </c>
@@ -2352,7 +2353,7 @@
         <v>110.376</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>32.619</v>
       </c>

</xml_diff>